<commit_message>
final results for all agents
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Ariel University\tesis\packmanGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dana\Desktop\Ariel University\tesis\packmanGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8354C464-F371-4FB6-921E-09D4C9EF2E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E472B7B-C7A6-40E7-91CD-306232A70FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3120" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="25">
   <si>
     <t>TSP</t>
   </si>
@@ -92,6 +89,27 @@
   <si>
     <t>computer value</t>
   </si>
+  <si>
+    <t>map 3:</t>
+  </si>
+  <si>
+    <t>computer_value</t>
+  </si>
+  <si>
+    <t>behavior</t>
+  </si>
+  <si>
+    <t>ddqn distribution v1</t>
+  </si>
+  <si>
+    <t>map 4:</t>
+  </si>
+  <si>
+    <t>map 5:</t>
+  </si>
+  <si>
+    <t>ddqn distribution v4</t>
+  </si>
 </sst>
 </file>
 
@@ -114,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -122,12 +140,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,114 +203,97 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="10">
-          <cell r="C10" t="str">
-            <v>Agent</v>
-          </cell>
-          <cell r="D10" t="str">
-            <v>Human</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Aggressive</v>
-          </cell>
-          <cell r="C11">
-            <v>-16.27</v>
-          </cell>
-          <cell r="D11">
-            <v>-18.399999999999999</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>Semi-aggressive</v>
-          </cell>
-          <cell r="C12">
-            <v>-60.96</v>
-          </cell>
-          <cell r="D12">
-            <v>-62.11</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>Careful</v>
-          </cell>
-          <cell r="C13">
-            <v>-2.29</v>
-          </cell>
-          <cell r="D13">
-            <v>-0.86</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>Random</v>
-          </cell>
-          <cell r="C14">
-            <v>-59.4</v>
-          </cell>
-          <cell r="D14">
-            <v>-57.62</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>Non-Velocity VI</v>
-          </cell>
-          <cell r="C15">
-            <v>-6.34</v>
-          </cell>
-          <cell r="D15">
-            <v>-9.0299999999999994</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>Velocity VI</v>
-          </cell>
-          <cell r="C16">
-            <v>-5.33</v>
-          </cell>
-          <cell r="D16">
-            <v>-6.03</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>Eq. Social VI</v>
-          </cell>
-          <cell r="C17">
-            <v>-2.35</v>
-          </cell>
-          <cell r="D17">
-            <v>-4.09</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>SARL</v>
-          </cell>
-          <cell r="C18">
-            <v>15.87</v>
-          </cell>
-          <cell r="D18">
-            <v>17.12</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>274504</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>7710</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D218E285-F92C-5FFF-3F91-D17295F9A42F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8526780" y="8305800"/>
+          <a:ext cx="2118544" cy="1044030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304988</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>91550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BA7536A-0B72-E60D-A41A-9C23723F277D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8511540" y="6697980"/>
+          <a:ext cx="2164268" cy="1272650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -518,13 +559,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:W69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J7" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="Q69" sqref="Q69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="14" max="14" width="17.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -751,11 +796,11 @@
         <v>0.82781066666666669</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10:R10" si="0">AVERAGE(D3, D12, D21)</f>
+        <f t="shared" ref="M10" si="0">AVERAGE(D3, D12, D21)</f>
         <v>0.86544433333333337</v>
       </c>
       <c r="N10">
-        <f>SUM(L10,M10)</f>
+        <f t="shared" ref="N10:N16" si="1">SUM(L10,M10)</f>
         <v>1.6932550000000002</v>
       </c>
     </row>
@@ -767,15 +812,15 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11:L15" si="1">AVERAGE(C4, C13, C22)</f>
+        <f t="shared" ref="L11:L14" si="2">AVERAGE(C4, C13, C22)</f>
         <v>0.69284000000000001</v>
       </c>
       <c r="M11">
-        <f t="shared" ref="M11:M15" si="2">AVERAGE(D4, D13, D22)</f>
+        <f t="shared" ref="M11:M15" si="3">AVERAGE(D4, D13, D22)</f>
         <v>0.78072966666666666</v>
       </c>
       <c r="N11">
-        <f>SUM(L11,M11)</f>
+        <f t="shared" si="1"/>
         <v>1.4735696666666667</v>
       </c>
     </row>
@@ -808,15 +853,15 @@
         <v>2</v>
       </c>
       <c r="L12">
+        <f t="shared" si="2"/>
+        <v>1.0976003333333333</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>0.10971599999999999</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="1"/>
-        <v>1.0976003333333333</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="2"/>
-        <v>0.10971599999999999</v>
-      </c>
-      <c r="N12">
-        <f>SUM(L12,M12)</f>
         <v>1.2073163333333332</v>
       </c>
     </row>
@@ -849,15 +894,15 @@
         <v>3</v>
       </c>
       <c r="L13">
+        <f t="shared" si="2"/>
+        <v>0.50217233333333333</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>0.52899033333333334</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="1"/>
-        <v>0.50217233333333333</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="2"/>
-        <v>0.52899033333333334</v>
-      </c>
-      <c r="N13">
-        <f>SUM(L13,M13)</f>
         <v>1.0311626666666667</v>
       </c>
     </row>
@@ -890,15 +935,15 @@
         <v>4</v>
       </c>
       <c r="L14">
+        <f t="shared" si="2"/>
+        <v>0.24250633333333335</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>0.24504466666666669</v>
+      </c>
+      <c r="N14">
         <f t="shared" si="1"/>
-        <v>0.24250633333333335</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="2"/>
-        <v>0.24504466666666669</v>
-      </c>
-      <c r="N14">
-        <f>SUM(L14,M14)</f>
         <v>0.48755100000000007</v>
       </c>
     </row>
@@ -935,11 +980,11 @@
         <v>1.1927599999999998</v>
       </c>
       <c r="M15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.63901166666666664</v>
       </c>
       <c r="N15">
-        <f>SUM(L15,M15)</f>
+        <f t="shared" si="1"/>
         <v>1.8317716666666666</v>
       </c>
     </row>
@@ -976,11 +1021,11 @@
         <v>1.1138620000000001</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16" si="3">AVERAGE(D9, D18, D27)</f>
+        <f t="shared" ref="M16" si="4">AVERAGE(D9, D18, D27)</f>
         <v>0.10520633333333336</v>
       </c>
       <c r="N16">
-        <f>SUM(L16,M16)</f>
+        <f t="shared" si="1"/>
         <v>1.2190683333333334</v>
       </c>
     </row>
@@ -1401,7 +1446,1166 @@
         <v>5.4736840000000004</v>
       </c>
     </row>
+    <row r="28" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="3"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" t="s">
+        <v>12</v>
+      </c>
+      <c r="J34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0.90897399999999995</v>
+      </c>
+      <c r="D35">
+        <v>0.97256399999999998</v>
+      </c>
+      <c r="F35">
+        <v>5.4871790000000003</v>
+      </c>
+      <c r="G35">
+        <v>5.3846150000000002</v>
+      </c>
+      <c r="H35">
+        <v>2.8974359999999999</v>
+      </c>
+      <c r="I35">
+        <v>5.7435900000000002</v>
+      </c>
+      <c r="J35">
+        <v>5.6923079999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0.75375000000000003</v>
+      </c>
+      <c r="D36">
+        <v>0.82250000000000001</v>
+      </c>
+      <c r="F36">
+        <v>4.9749999999999996</v>
+      </c>
+      <c r="G36">
+        <v>5.0750000000000002</v>
+      </c>
+      <c r="H36">
+        <v>3.5249999999999999</v>
+      </c>
+      <c r="I36">
+        <v>4.75</v>
+      </c>
+      <c r="J36">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>0.30361100000000002</v>
+      </c>
+      <c r="D37">
+        <v>0.46777800000000003</v>
+      </c>
+      <c r="F37">
+        <v>3.4166669999999999</v>
+      </c>
+      <c r="G37">
+        <v>4.3888889999999998</v>
+      </c>
+      <c r="H37">
+        <v>4.75</v>
+      </c>
+      <c r="I37">
+        <v>3.2222219999999999</v>
+      </c>
+      <c r="J37">
+        <v>5.8888889999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>1.0615619999999999</v>
+      </c>
+      <c r="D38">
+        <v>0.15593799999999999</v>
+      </c>
+      <c r="F38">
+        <v>2.125</v>
+      </c>
+      <c r="G38">
+        <v>5.625</v>
+      </c>
+      <c r="H38">
+        <v>6.21875</v>
+      </c>
+      <c r="I38">
+        <v>3.625</v>
+      </c>
+      <c r="J38">
+        <v>5.96875</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>0.30019600000000002</v>
+      </c>
+      <c r="D39">
+        <v>0.34921600000000003</v>
+      </c>
+      <c r="F39">
+        <v>2.7647059999999999</v>
+      </c>
+      <c r="G39">
+        <v>3.803922</v>
+      </c>
+      <c r="H39">
+        <v>5.2156859999999998</v>
+      </c>
+      <c r="I39">
+        <v>3.058824</v>
+      </c>
+      <c r="J39">
+        <v>5.9607840000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>1.0615619999999999</v>
+      </c>
+      <c r="D40">
+        <v>0.15593799999999999</v>
+      </c>
+      <c r="F40">
+        <v>2.125</v>
+      </c>
+      <c r="G40">
+        <v>5.625</v>
+      </c>
+      <c r="H40">
+        <v>6.21875</v>
+      </c>
+      <c r="I40">
+        <v>3.625</v>
+      </c>
+      <c r="J40">
+        <v>5.96875</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>1.141316</v>
+      </c>
+      <c r="D41">
+        <v>0.781053</v>
+      </c>
+      <c r="F41">
+        <v>4.9736840000000004</v>
+      </c>
+      <c r="G41">
+        <v>5.4210529999999997</v>
+      </c>
+      <c r="H41">
+        <v>5.3157889999999997</v>
+      </c>
+      <c r="I41">
+        <v>5.3421050000000001</v>
+      </c>
+      <c r="J41">
+        <v>5.447368</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42">
+        <v>1.076222</v>
+      </c>
+      <c r="D42">
+        <v>0.66755600000000004</v>
+      </c>
+      <c r="F42">
+        <v>4.3111110000000004</v>
+      </c>
+      <c r="G42">
+        <v>4.5777780000000003</v>
+      </c>
+      <c r="H42">
+        <v>4.2444439999999997</v>
+      </c>
+      <c r="I42">
+        <v>4.8666669999999996</v>
+      </c>
+      <c r="J42">
+        <v>5.5111109999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43">
+        <v>1.0615619999999999</v>
+      </c>
+      <c r="D43">
+        <v>0.15593799999999999</v>
+      </c>
+      <c r="F43">
+        <v>2.125</v>
+      </c>
+      <c r="G43">
+        <v>5.625</v>
+      </c>
+      <c r="H43">
+        <v>6.21875</v>
+      </c>
+      <c r="I43">
+        <v>3.625</v>
+      </c>
+      <c r="J43">
+        <v>5.96875</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0.88</v>
+      </c>
+      <c r="D48">
+        <v>0.88314300000000001</v>
+      </c>
+      <c r="F48">
+        <v>4.7428569999999999</v>
+      </c>
+      <c r="G48">
+        <v>4.8</v>
+      </c>
+      <c r="H48">
+        <v>3.6</v>
+      </c>
+      <c r="I48">
+        <v>5.8</v>
+      </c>
+      <c r="J48">
+        <v>5.0857140000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>0.90106399999999998</v>
+      </c>
+      <c r="D49">
+        <v>0.93085099999999998</v>
+      </c>
+      <c r="F49">
+        <v>4.9148940000000003</v>
+      </c>
+      <c r="G49">
+        <v>5.0638300000000003</v>
+      </c>
+      <c r="H49">
+        <v>3.851064</v>
+      </c>
+      <c r="I49">
+        <v>5.553191</v>
+      </c>
+      <c r="J49">
+        <v>5.595745</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>0.605128</v>
+      </c>
+      <c r="D50">
+        <v>0.668462</v>
+      </c>
+      <c r="F50">
+        <v>4.7948719999999998</v>
+      </c>
+      <c r="G50">
+        <v>5.0512819999999996</v>
+      </c>
+      <c r="H50">
+        <v>5.1538459999999997</v>
+      </c>
+      <c r="I50">
+        <v>5.2307689999999996</v>
+      </c>
+      <c r="J50">
+        <v>5.461538</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51">
+        <v>1.180444</v>
+      </c>
+      <c r="D51">
+        <v>0.372444</v>
+      </c>
+      <c r="F51">
+        <v>3.5333329999999998</v>
+      </c>
+      <c r="G51">
+        <v>5.2444439999999997</v>
+      </c>
+      <c r="H51">
+        <v>6.088889</v>
+      </c>
+      <c r="I51">
+        <v>4.0444440000000004</v>
+      </c>
+      <c r="J51">
+        <v>5.3111110000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>0.402619</v>
+      </c>
+      <c r="D52">
+        <v>0.48714299999999999</v>
+      </c>
+      <c r="F52">
+        <v>4.0952380000000002</v>
+      </c>
+      <c r="G52">
+        <v>5</v>
+      </c>
+      <c r="H52">
+        <v>5.7142860000000004</v>
+      </c>
+      <c r="I52">
+        <v>4.4523809999999999</v>
+      </c>
+      <c r="J52">
+        <v>5.4047619999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>1.180444</v>
+      </c>
+      <c r="D53">
+        <v>0.372444</v>
+      </c>
+      <c r="F53">
+        <v>3.5333329999999998</v>
+      </c>
+      <c r="G53">
+        <v>5.2444439999999997</v>
+      </c>
+      <c r="H53">
+        <v>6.088889</v>
+      </c>
+      <c r="I53">
+        <v>4.0444440000000004</v>
+      </c>
+      <c r="J53">
+        <v>5.3111110000000004</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54">
+        <v>1.180444</v>
+      </c>
+      <c r="D54">
+        <v>0.372444</v>
+      </c>
+      <c r="F54">
+        <v>3.5333329999999998</v>
+      </c>
+      <c r="G54">
+        <v>5.2444439999999997</v>
+      </c>
+      <c r="H54">
+        <v>6.088889</v>
+      </c>
+      <c r="I54">
+        <v>4.0444440000000004</v>
+      </c>
+      <c r="J54">
+        <v>5.3111110000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55">
+        <v>1.180444</v>
+      </c>
+      <c r="D55">
+        <v>0.372444</v>
+      </c>
+      <c r="F55">
+        <v>3.5333329999999998</v>
+      </c>
+      <c r="G55">
+        <v>5.2444439999999997</v>
+      </c>
+      <c r="H55">
+        <v>6.088889</v>
+      </c>
+      <c r="I55">
+        <v>4.0444440000000004</v>
+      </c>
+      <c r="J55">
+        <v>5.3111110000000004</v>
+      </c>
+      <c r="O55" t="s">
+        <v>7</v>
+      </c>
+      <c r="P55" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>16</v>
+      </c>
+      <c r="S55" t="s">
+        <v>9</v>
+      </c>
+      <c r="T55" t="s">
+        <v>10</v>
+      </c>
+      <c r="U55" t="s">
+        <v>11</v>
+      </c>
+      <c r="V55" t="s">
+        <v>12</v>
+      </c>
+      <c r="W55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56">
+        <v>1.180444</v>
+      </c>
+      <c r="D56">
+        <v>0.372444</v>
+      </c>
+      <c r="F56">
+        <v>3.5333329999999998</v>
+      </c>
+      <c r="G56">
+        <v>5.2444439999999997</v>
+      </c>
+      <c r="H56">
+        <v>6.088889</v>
+      </c>
+      <c r="I56">
+        <v>4.0444440000000004</v>
+      </c>
+      <c r="J56">
+        <v>5.3111110000000004</v>
+      </c>
+      <c r="N56" t="s">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <f>AVERAGE(C35, C48, C61)</f>
+        <v>0.83680100000000002</v>
+      </c>
+      <c r="P56">
+        <f>AVERAGE(D35, D48, D61)</f>
+        <v>0.88516766666666669</v>
+      </c>
+      <c r="Q56">
+        <f>SUM(O56,P56)</f>
+        <v>1.7219686666666667</v>
+      </c>
+      <c r="S56">
+        <f>AVERAGE(F35, F48, F61)</f>
+        <v>4.9542296666666665</v>
+      </c>
+      <c r="T56">
+        <f>AVERAGE(G35, G48, G61)</f>
+        <v>5.0547356666666667</v>
+      </c>
+      <c r="U56">
+        <f>AVERAGE(H35, H48, H61)</f>
+        <v>3.3018663333333333</v>
+      </c>
+      <c r="V56">
+        <f>AVERAGE(I35, I48, I61)</f>
+        <v>5.5825573333333338</v>
+      </c>
+      <c r="W56">
+        <f>AVERAGE(J35, J48, J61)</f>
+        <v>5.2729460000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="N57" t="s">
+        <v>1</v>
+      </c>
+      <c r="O57">
+        <f t="shared" ref="O57:P57" si="5">AVERAGE(C36, C49, C62)</f>
+        <v>0.73556699999999997</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="5"/>
+        <v>0.80476466666666668</v>
+      </c>
+      <c r="Q57">
+        <f>SUM(O57,P57)</f>
+        <v>1.5403316666666667</v>
+      </c>
+      <c r="S57">
+        <f>AVERAGE(F36, F49, F62)</f>
+        <v>4.5985179999999994</v>
+      </c>
+      <c r="T57">
+        <f>AVERAGE(G36, G49, G62)</f>
+        <v>5.1091696666666664</v>
+      </c>
+      <c r="U57">
+        <f>AVERAGE(H36, H49, H62)</f>
+        <v>3.7542853333333333</v>
+      </c>
+      <c r="V57">
+        <f>AVERAGE(I36, I49, I62)</f>
+        <v>5.2142713333333335</v>
+      </c>
+      <c r="W57">
+        <f>AVERAGE(J36, J49, J62)</f>
+        <v>5.5655626666666675</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="N58" t="s">
+        <v>3</v>
+      </c>
+      <c r="O58">
+        <f t="shared" ref="O58:P58" si="6">AVERAGE(C37, C50, C63)</f>
+        <v>0.55196866666666666</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="6"/>
+        <v>0.58619100000000002</v>
+      </c>
+      <c r="Q58">
+        <f>SUM(O58,P58)</f>
+        <v>1.1381596666666667</v>
+      </c>
+      <c r="S58">
+        <f>AVERAGE(F37, F50, F63)</f>
+        <v>4.1816240000000002</v>
+      </c>
+      <c r="T58">
+        <f>AVERAGE(G37, G50, G63)</f>
+        <v>4.6300569999999999</v>
+      </c>
+      <c r="U58">
+        <f>AVERAGE(H37, H50, H63)</f>
+        <v>4.529059666666666</v>
+      </c>
+      <c r="V58">
+        <f>AVERAGE(I37, I50, I63)</f>
+        <v>4.4843303333333333</v>
+      </c>
+      <c r="W58">
+        <f>AVERAGE(J37, J50, J63)</f>
+        <v>5.3779199999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="N59" t="s">
+        <v>6</v>
+      </c>
+      <c r="O59">
+        <f t="shared" ref="O59:P59" si="7">AVERAGE(C38, C51, C64)</f>
+        <v>1.1190020000000001</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="7"/>
+        <v>0.141544</v>
+      </c>
+      <c r="Q59">
+        <f>SUM(O59,P59)</f>
+        <v>1.2605460000000002</v>
+      </c>
+      <c r="S59">
+        <f>AVERAGE(F38, F51, F64)</f>
+        <v>2.9444443333333332</v>
+      </c>
+      <c r="T59">
+        <f>AVERAGE(G38, G51, G64)</f>
+        <v>5.1148146666666667</v>
+      </c>
+      <c r="U59">
+        <f>AVERAGE(H38, H51, H64)</f>
+        <v>5.7942130000000001</v>
+      </c>
+      <c r="V59">
+        <f>AVERAGE(I38, I51, I64)</f>
+        <v>3.9898146666666663</v>
+      </c>
+      <c r="W59">
+        <f>AVERAGE(J38, J51, J64)</f>
+        <v>5.4099536666666665</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" t="s">
+        <v>10</v>
+      </c>
+      <c r="H60" t="s">
+        <v>11</v>
+      </c>
+      <c r="I60" t="s">
+        <v>12</v>
+      </c>
+      <c r="J60" t="s">
+        <v>19</v>
+      </c>
+      <c r="N60" t="s">
+        <v>4</v>
+      </c>
+      <c r="O60">
+        <f t="shared" ref="O60:P60" si="8">AVERAGE(C39, C52, C65)</f>
+        <v>0.2179523333333333</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="8"/>
+        <v>0.23663366666666671</v>
+      </c>
+      <c r="Q60">
+        <f>SUM(O60,P60)</f>
+        <v>0.45458600000000005</v>
+      </c>
+      <c r="S60">
+        <f>AVERAGE(F39, F52, F65)</f>
+        <v>3.3977590000000002</v>
+      </c>
+      <c r="T60">
+        <f>AVERAGE(G39, G52, G65)</f>
+        <v>4.4624183333333329</v>
+      </c>
+      <c r="U60">
+        <f>AVERAGE(H39, H52, H65)</f>
+        <v>5.1433239999999998</v>
+      </c>
+      <c r="V60">
+        <f>AVERAGE(I39, I52, I65)</f>
+        <v>3.6912350000000003</v>
+      </c>
+      <c r="W60">
+        <f>AVERAGE(J39, J52, J65)</f>
+        <v>5.4135153333333337</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0.72142899999999999</v>
+      </c>
+      <c r="D61">
+        <v>0.79979599999999995</v>
+      </c>
+      <c r="F61">
+        <v>4.6326530000000004</v>
+      </c>
+      <c r="G61">
+        <v>4.9795920000000002</v>
+      </c>
+      <c r="H61">
+        <v>3.4081630000000001</v>
+      </c>
+      <c r="I61">
+        <v>5.2040819999999997</v>
+      </c>
+      <c r="J61">
+        <v>5.0408160000000004</v>
+      </c>
+      <c r="N61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O61">
+        <f t="shared" ref="O61:P61" si="9">AVERAGE(C40, C53, C66)</f>
+        <v>1.106908</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="9"/>
+        <v>0.125529</v>
+      </c>
+      <c r="Q61">
+        <f>SUM(O61,P61)</f>
+        <v>1.232437</v>
+      </c>
+      <c r="S61">
+        <f>AVERAGE(F40, F53, F66)</f>
+        <v>3.0570513333333333</v>
+      </c>
+      <c r="T61">
+        <f>AVERAGE(G40, G53, G66)</f>
+        <v>5.4436606666666663</v>
+      </c>
+      <c r="U61">
+        <f>AVERAGE(H40, H53, H66)</f>
+        <v>6.1367343333333331</v>
+      </c>
+      <c r="V61">
+        <f>AVERAGE(I40, I53, I66)</f>
+        <v>3.9154556666666664</v>
+      </c>
+      <c r="W61">
+        <f>AVERAGE(J40, J53, J66)</f>
+        <v>5.5633723333333336</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>0.55188700000000002</v>
+      </c>
+      <c r="D62">
+        <v>0.66094299999999995</v>
+      </c>
+      <c r="F62">
+        <v>3.9056600000000001</v>
+      </c>
+      <c r="G62">
+        <v>5.1886789999999996</v>
+      </c>
+      <c r="H62">
+        <v>3.8867919999999998</v>
+      </c>
+      <c r="I62">
+        <v>5.3396229999999996</v>
+      </c>
+      <c r="J62">
+        <v>5.1509429999999998</v>
+      </c>
+      <c r="N62" t="s">
+        <v>5</v>
+      </c>
+      <c r="O62">
+        <f>AVERAGE(C8, C17, C26)</f>
+        <v>1.1927599999999998</v>
+      </c>
+      <c r="P62">
+        <f t="shared" ref="P62:Q62" si="10">AVERAGE(D8, D17, D26)</f>
+        <v>0.63901166666666664</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="10"/>
+        <v>3.7609133333333333</v>
+      </c>
+      <c r="S62">
+        <f>AVERAGE(F41, F54, F67)</f>
+        <v>4.256307333333333</v>
+      </c>
+      <c r="T62">
+        <f>AVERAGE(G41, G54, G67)</f>
+        <v>5.2059593333333325</v>
+      </c>
+      <c r="U62">
+        <f>AVERAGE(H41, H54, H67)</f>
+        <v>5.6031466666666674</v>
+      </c>
+      <c r="V62">
+        <f>AVERAGE(I41, I54, I67)</f>
+        <v>4.7637703333333334</v>
+      </c>
+      <c r="W62">
+        <f>AVERAGE(J41, J54, J67)</f>
+        <v>5.4433026666666677</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63">
+        <v>0.74716700000000003</v>
+      </c>
+      <c r="D63">
+        <v>0.62233300000000003</v>
+      </c>
+      <c r="F63">
+        <v>4.3333329999999997</v>
+      </c>
+      <c r="G63">
+        <v>4.45</v>
+      </c>
+      <c r="H63">
+        <v>3.6833330000000002</v>
+      </c>
+      <c r="I63">
+        <v>5</v>
+      </c>
+      <c r="J63">
+        <v>4.7833329999999998</v>
+      </c>
+      <c r="N63" t="s">
+        <v>21</v>
+      </c>
+      <c r="O63">
+        <f>AVERAGE(C42, C55, C68)</f>
+        <v>1.1007406666666666</v>
+      </c>
+      <c r="P63">
+        <f t="shared" ref="O63:P63" si="11">AVERAGE(D42, D55, D68)</f>
+        <v>0.48311100000000001</v>
+      </c>
+      <c r="Q63">
+        <f>SUM(O63,P63)</f>
+        <v>1.5838516666666667</v>
+      </c>
+      <c r="S63">
+        <f>AVERAGE(F42, F55, F68)</f>
+        <v>3.8814813333333333</v>
+      </c>
+      <c r="T63">
+        <f>AVERAGE(G42, G55, G68)</f>
+        <v>4.6888886666666663</v>
+      </c>
+      <c r="U63">
+        <f>AVERAGE(H42, H55, H68)</f>
+        <v>4.9481479999999998</v>
+      </c>
+      <c r="V63">
+        <f>AVERAGE(I42, I55, I68)</f>
+        <v>4.429629666666667</v>
+      </c>
+      <c r="W63">
+        <f>AVERAGE(J42, J55, J68)</f>
+        <v>5.3111110000000004</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64">
+        <v>1.115</v>
+      </c>
+      <c r="D64">
+        <v>-0.10375</v>
+      </c>
+      <c r="F64">
+        <v>3.1749999999999998</v>
+      </c>
+      <c r="G64">
+        <v>4.4749999999999996</v>
+      </c>
+      <c r="H64">
+        <v>5.0750000000000002</v>
+      </c>
+      <c r="I64">
+        <v>4.3</v>
+      </c>
+      <c r="J64">
+        <v>4.95</v>
+      </c>
+      <c r="N64" t="s">
+        <v>24</v>
+      </c>
+      <c r="O64">
+        <f t="shared" ref="O64:P64" si="12">AVERAGE(C43, C56, C69)</f>
+        <v>1.0930929999999999</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="12"/>
+        <v>0.37946066666666667</v>
+      </c>
+      <c r="Q64">
+        <f>SUM(O64,P64)</f>
+        <v>1.4725536666666665</v>
+      </c>
+      <c r="S64">
+        <f>AVERAGE(F43, F56, F69)</f>
+        <v>3.4012626666666663</v>
+      </c>
+      <c r="T64">
+        <f>AVERAGE(G43, G56, G69)</f>
+        <v>5.2216329999999997</v>
+      </c>
+      <c r="U64">
+        <f>AVERAGE(H43, H56, H69)</f>
+        <v>5.7464856666666675</v>
+      </c>
+      <c r="V64">
+        <f>AVERAGE(I43, I56, I69)</f>
+        <v>4.09436</v>
+      </c>
+      <c r="W64">
+        <f>AVERAGE(J43, J56, J69)</f>
+        <v>5.4493476666666671</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65">
+        <v>-4.8958000000000002E-2</v>
+      </c>
+      <c r="D65">
+        <v>-0.12645799999999999</v>
+      </c>
+      <c r="F65">
+        <v>3.3333330000000001</v>
+      </c>
+      <c r="G65">
+        <v>4.5833329999999997</v>
+      </c>
+      <c r="H65">
+        <v>4.5</v>
+      </c>
+      <c r="I65">
+        <v>3.5625</v>
+      </c>
+      <c r="J65">
+        <v>4.875</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <v>1.0787180000000001</v>
+      </c>
+      <c r="D66">
+        <v>-0.15179500000000001</v>
+      </c>
+      <c r="F66">
+        <v>3.5128210000000002</v>
+      </c>
+      <c r="G66">
+        <v>5.461538</v>
+      </c>
+      <c r="H66">
+        <v>6.1025640000000001</v>
+      </c>
+      <c r="I66">
+        <v>4.0769229999999999</v>
+      </c>
+      <c r="J66">
+        <v>5.4102560000000004</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <v>1.1723809999999999</v>
+      </c>
+      <c r="D67">
+        <v>0.64904799999999996</v>
+      </c>
+      <c r="F67">
+        <v>4.2619049999999996</v>
+      </c>
+      <c r="G67">
+        <v>4.9523809999999999</v>
+      </c>
+      <c r="H67">
+        <v>5.4047619999999998</v>
+      </c>
+      <c r="I67">
+        <v>4.9047619999999998</v>
+      </c>
+      <c r="J67">
+        <v>5.5714290000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68">
+        <v>1.0455559999999999</v>
+      </c>
+      <c r="D68">
+        <v>0.409333</v>
+      </c>
+      <c r="F68">
+        <v>3.8</v>
+      </c>
+      <c r="G68">
+        <v>4.2444439999999997</v>
+      </c>
+      <c r="H68">
+        <v>4.5111109999999996</v>
+      </c>
+      <c r="I68">
+        <v>4.3777780000000002</v>
+      </c>
+      <c r="J68">
+        <v>5.1111110000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69">
+        <v>1.0372729999999999</v>
+      </c>
+      <c r="D69">
+        <v>0.61</v>
+      </c>
+      <c r="F69">
+        <v>4.5454549999999996</v>
+      </c>
+      <c r="G69">
+        <v>4.7954549999999996</v>
+      </c>
+      <c r="H69">
+        <v>4.9318179999999998</v>
+      </c>
+      <c r="I69">
+        <v>4.6136359999999996</v>
+      </c>
+      <c r="J69">
+        <v>5.0681820000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>